<commit_message>
Product count parsing from order sheet
</commit_message>
<xml_diff>
--- a/api/order/sample-order-v070420.xlsx
+++ b/api/order/sample-order-v070420.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="99">
   <si>
     <t xml:space="preserve">Village Greens Order Form</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Email</t>
   </si>
   <si>
-    <t xml:space="preserve">Dev-farmbox99@howapped.com</t>
+    <t xml:space="preserve">Dev+farmbox99@howapped.com</t>
   </si>
   <si>
     <t xml:space="preserve">Phone Number</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">Avocado : Ripe ready to eat</t>
   </si>
   <si>
-    <t xml:space="preserve">one</t>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">Baby Leaf Salad Bag</t>
@@ -262,9 +262,6 @@
     <t xml:space="preserve">Lemon</t>
   </si>
   <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lime</t>
   </si>
   <si>
@@ -284,9 +281,6 @@
   </si>
   <si>
     <t xml:space="preserve">Strawberries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 punnets please!</t>
   </si>
   <si>
     <t xml:space="preserve">Milk </t>
@@ -361,7 +355,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="\£#,##0.00"/>
     <numFmt numFmtId="167" formatCode="\£#,##0.00;[RED]&quot;-£&quot;#,##0.00"/>
   </numFmts>
@@ -478,6 +472,7 @@
       <color rgb="FF3D3D3D"/>
       <name val="Ubuntu"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -853,12 +848,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -925,7 +920,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1476360</xdr:colOff>
@@ -934,9 +929,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2294640</xdr:colOff>
+      <xdr:colOff>2293560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>637200</xdr:rowOff>
+      <xdr:rowOff>636120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -950,7 +945,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5307840" y="9360"/>
-          <a:ext cx="818280" cy="627840"/>
+          <a:ext cx="817200" cy="626760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -970,19 +965,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A69" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C69" activeCellId="0" sqref="C69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="0" width="7.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="12.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2522,7 +2518,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D54" s="26" t="n">
         <v>0.4</v>
@@ -2552,7 +2548,7 @@
     </row>
     <row r="55" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" s="21" t="n">
         <v>1</v>
@@ -2586,7 +2582,7 @@
     </row>
     <row r="56" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" s="21" t="n">
         <v>1</v>
@@ -2620,10 +2616,10 @@
     </row>
     <row r="57" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="21" t="s">
         <v>73</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>74</v>
       </c>
       <c r="C57" s="21"/>
       <c r="D57" s="26" t="n">
@@ -2654,10 +2650,10 @@
     </row>
     <row r="58" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="21" t="s">
         <v>75</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>76</v>
       </c>
       <c r="C58" s="21" t="n">
         <v>1</v>
@@ -2690,13 +2686,13 @@
     </row>
     <row r="59" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B59" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="21" t="s">
-        <v>78</v>
+      <c r="C59" s="21" t="n">
+        <v>2</v>
       </c>
       <c r="D59" s="26" t="n">
         <v>1.95</v>
@@ -2754,7 +2750,7 @@
     </row>
     <row r="61" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B61" s="35"/>
       <c r="C61" s="21"/>
@@ -2812,7 +2808,7 @@
     </row>
     <row r="63" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B63" s="21" t="n">
         <v>1</v>
@@ -2846,7 +2842,7 @@
     </row>
     <row r="64" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
@@ -2878,7 +2874,7 @@
     </row>
     <row r="65" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B65" s="21" t="n">
         <v>1</v>
@@ -2912,7 +2908,7 @@
     </row>
     <row r="66" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B66" s="21" t="n">
         <v>1</v>
@@ -2946,7 +2942,7 @@
     </row>
     <row r="67" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B67" s="21" t="n">
         <v>1</v>
@@ -2980,7 +2976,7 @@
     </row>
     <row r="68" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B68" s="21" t="n">
         <v>1</v>
@@ -3014,7 +3010,7 @@
     </row>
     <row r="69" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B69" s="21" t="n">
         <v>1</v>
@@ -3048,7 +3044,7 @@
     </row>
     <row r="70" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B70" s="21" t="n">
         <v>1</v>
@@ -3084,7 +3080,7 @@
     </row>
     <row r="71" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B71" s="21" t="n">
         <v>1</v>
@@ -3118,7 +3114,7 @@
     </row>
     <row r="72" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B72" s="21" t="n">
         <v>1</v>
@@ -3150,7 +3146,7 @@
     </row>
     <row r="73" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B73" s="21" t="n">
         <v>1</v>
@@ -3184,7 +3180,7 @@
     </row>
     <row r="74" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B74" s="21" t="n">
         <v>1</v>
@@ -3218,7 +3214,7 @@
     </row>
     <row r="75" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B75" s="21" t="n">
         <v>1</v>
@@ -3252,7 +3248,7 @@
     </row>
     <row r="76" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B76" s="21" t="n">
         <v>1</v>
@@ -3286,7 +3282,7 @@
     </row>
     <row r="77" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B77" s="21" t="n">
         <v>1</v>
@@ -3320,7 +3316,7 @@
     </row>
     <row r="78" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B78" s="21" t="n">
         <v>1</v>
@@ -3354,7 +3350,7 @@
     </row>
     <row r="79" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B79" s="21" t="n">
         <v>1</v>
@@ -3388,7 +3384,7 @@
     </row>
     <row r="80" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B80" s="21" t="n">
         <v>1</v>
@@ -3422,7 +3418,7 @@
     </row>
     <row r="81" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B81" s="21" t="n">
         <v>1</v>
@@ -3456,13 +3452,13 @@
     </row>
     <row r="82" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B82" s="21" t="n">
         <v>1</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D82" s="39" t="n">
         <v>6.15</v>

</xml_diff>

<commit_message>
Log Order Form reader exceptions to the DB for debugging from Django Admin
</commit_message>
<xml_diff>
--- a/api/order/sample-order-v070420.xlsx
+++ b/api/order/sample-order-v070420.xlsx
@@ -929,9 +929,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2293560</xdr:colOff>
+      <xdr:colOff>2293200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>636120</xdr:rowOff>
+      <xdr:rowOff>635760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -945,7 +945,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5307840" y="9360"/>
-          <a:ext cx="817200" cy="626760"/>
+          <a:ext cx="816840" cy="626400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -967,8 +967,8 @@
   </sheetPr>
   <dimension ref="A1:Z84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>